<commit_message>
modified:   products.php 	modified:   products/template.php 	modified:   samplefile/ZoovuSampleData.xlsx
</commit_message>
<xml_diff>
--- a/samplefile/ZoovuSampleData.xlsx
+++ b/samplefile/ZoovuSampleData.xlsx
@@ -5,22 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexHackman\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ZoovuDemoShop\ahackman\samplefile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CE1A341-B483-4736-A6B7-E54B5BCA2413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654D18B7-237E-4B20-95FB-0852D5AF2B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="183">
   <si>
     <t>Name</t>
   </si>
@@ -494,13 +507,88 @@
   </si>
   <si>
     <t>Smart, Energy Star Certified</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/c9988a81-6225-495e-9916-63507b5d2d52</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/f9ede074-9c83-410f-afc0-5b3ada0d4856</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/ddf8cab7-b0a1-4472-b4ad-e5b8c1668ede</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/6de2fc55-1be4-4be6-bd5d-96563927d2cc</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/6cfe5cbe-7a63-4113-a69f-cfaf03613f33</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/c9988a81-6225-495e-9916-63507b5d2d53</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/f9ede074-9c83-410f-afc0-5b3ada0d4857</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/132b01cc-9c95-4892-912f-64e65c2a71d0</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/21bd4264-0b81-4daa-af12-c49864d722a2</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/05a85fa1-5d00-4149-b119-50b4d9900baf</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/26e83aa3-73e4-4861-861b-2336ff73a757</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/132b01cc-9c95-4892-912f-64e65c2a71d1</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/21bd4264-0b81-4daa-af12-c49864d722a3</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/42823f08-0426-43ea-bd7b-39bc9cd0a001</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/fac7f86a-c529-4e61-9606-8d1792f57276</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/138255fa-5f8c-48ab-baa2-ff10b2a19b98</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/410eb56b-b1b6-48e7-9d66-de64912d72dc</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/42823f08-0426-43ea-bd7b-39bc9cd0a002</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/fac7f86a-c529-4e61-9606-8d1792f57277</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/138255fa-5f8c-48ab-baa2-ff10b2a19b99</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/42823f08-0426-43ea-bd7b-39bc9cd0a003</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/39b17a36-41ef-4b7c-be2d-772a1f4ae6e5</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/9695a092-bc82-432a-92b8-e1f0d34be95d</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/81000d59-9d12-4ec7-a7c4-fc3d7328d5cb</t>
+  </si>
+  <si>
+    <t>https://assets-barracuda-zoovu.azureedge.net/zoovu/8bf3c049-944c-4886-bd36-56ef54258628</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -536,6 +624,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -560,10 +655,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -574,8 +670,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -795,12 +893,13 @@
   <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="2" max="3" width="12.6640625" customWidth="1"/>
     <col min="6" max="9" width="12.6640625" style="4"/>
   </cols>
   <sheetData>
@@ -873,8 +972,8 @@
       <c r="C2" s="1">
         <v>549</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
+      <c r="D2" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>17</v>
@@ -932,8 +1031,8 @@
       <c r="C3" s="1">
         <v>699</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
+      <c r="D3" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>17</v>
@@ -991,8 +1090,8 @@
       <c r="C4" s="1">
         <v>1199</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
+      <c r="D4" s="6" t="s">
+        <v>167</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>17</v>
@@ -1050,8 +1149,8 @@
       <c r="C5" s="1">
         <v>1299</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
+      <c r="D5" s="6" t="s">
+        <v>168</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>17</v>
@@ -1109,8 +1208,8 @@
       <c r="C6" s="1">
         <v>499</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
+      <c r="D6" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>17</v>
@@ -1168,8 +1267,8 @@
       <c r="C7" s="1">
         <v>549</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>17</v>
+      <c r="D7" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>17</v>
@@ -1227,8 +1326,8 @@
       <c r="C8" s="1">
         <v>799</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>17</v>
+      <c r="D8" s="6" t="s">
+        <v>167</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>17</v>
@@ -1286,8 +1385,8 @@
       <c r="C9" s="1">
         <v>1299</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>17</v>
+      <c r="D9" s="6" t="s">
+        <v>171</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>17</v>
@@ -1342,8 +1441,8 @@
       <c r="C10" s="1">
         <v>1499</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>17</v>
+      <c r="D10" s="6" t="s">
+        <v>172</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>17</v>
@@ -1401,8 +1500,8 @@
       <c r="C11" s="1">
         <v>1299</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>17</v>
+      <c r="D11" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>17</v>
@@ -1460,8 +1559,8 @@
       <c r="C12" s="1">
         <v>1599</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>17</v>
+      <c r="D12" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>17</v>
@@ -1516,8 +1615,8 @@
       <c r="C13" s="1">
         <v>1599</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>17</v>
+      <c r="D13" s="6" t="s">
+        <v>175</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>17</v>
@@ -1575,8 +1674,8 @@
       <c r="C14" s="1">
         <v>1199</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>17</v>
+      <c r="D14" s="6" t="s">
+        <v>176</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>17</v>
@@ -1634,8 +1733,8 @@
       <c r="C15" s="1">
         <v>1599</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>17</v>
+      <c r="D15" s="6" t="s">
+        <v>177</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>17</v>
@@ -1690,8 +1789,8 @@
       <c r="C16" s="1">
         <v>1499</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>17</v>
+      <c r="D16" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>17</v>
@@ -1749,8 +1848,8 @@
       <c r="C17" s="1">
         <v>1199</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>17</v>
+      <c r="D17" s="6" t="s">
+        <v>178</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>17</v>
@@ -1808,8 +1907,8 @@
       <c r="C18" s="1">
         <v>449</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>17</v>
+      <c r="D18" s="6" t="s">
+        <v>158</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>17</v>
@@ -1867,8 +1966,8 @@
       <c r="C19" s="1">
         <v>499</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>17</v>
+      <c r="D19" s="6" t="s">
+        <v>159</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>17</v>
@@ -1926,8 +2025,8 @@
       <c r="C20" s="1">
         <v>499</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>17</v>
+      <c r="D20" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>17</v>
@@ -1979,8 +2078,8 @@
       <c r="C21" s="1">
         <v>699</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>17</v>
+      <c r="D21" s="6" t="s">
+        <v>161</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>17</v>
@@ -2038,8 +2137,8 @@
       <c r="C22" s="1">
         <v>599</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>17</v>
+      <c r="D22" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>17</v>
@@ -2097,8 +2196,8 @@
       <c r="C23" s="1">
         <v>699</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>17</v>
+      <c r="D23" s="6" t="s">
+        <v>163</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>17</v>
@@ -2150,8 +2249,8 @@
       <c r="C24" s="1">
         <v>449</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>17</v>
+      <c r="D24" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>17</v>
@@ -2209,8 +2308,8 @@
       <c r="C25" s="1">
         <v>499</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>17</v>
+      <c r="D25" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>17</v>
@@ -2268,8 +2367,8 @@
       <c r="C26" s="1">
         <v>499</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>17</v>
+      <c r="D26" s="6" t="s">
+        <v>161</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>17</v>
@@ -2321,8 +2420,8 @@
       <c r="C27" s="1">
         <v>199</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>17</v>
+      <c r="D27" s="6" t="s">
+        <v>179</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>17</v>
@@ -2380,8 +2479,8 @@
       <c r="C28" s="1">
         <v>249</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>17</v>
+      <c r="D28" s="6" t="s">
+        <v>180</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>17</v>
@@ -2439,8 +2538,8 @@
       <c r="C29" s="1">
         <v>399</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>17</v>
+      <c r="D29" s="6" t="s">
+        <v>181</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>17</v>
@@ -2498,8 +2597,8 @@
       <c r="C30" s="1">
         <v>349</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>17</v>
+      <c r="D30" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>17</v>
@@ -2550,64 +2649,64 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D6" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="D8" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E8" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="D9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E9" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="D10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E10" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="D11" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E30" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="E29" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="E28" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="E27" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="E26" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="E25" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="E24" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="E23" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="E22" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="E21" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="E20" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="E19" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="E18" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="E15" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E14" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E13" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E12" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="E11" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="D12" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="E12" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="D13" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="E13" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="D14" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="E14" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="D15" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="E15" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="D16" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="E16" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="D17" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="E17" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="D18" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="E18" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="D19" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="E19" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="D20" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="E20" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="D21" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="E21" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="D22" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="E22" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="D23" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="E23" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="D24" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="E24" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="D25" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="E25" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="D26" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="E26" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="D27" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="E27" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="D28" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="E28" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="D29" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="E29" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="D30" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="E30" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="E10" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E9" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E8" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E7" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E6" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E5" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E4" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E3" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E2" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D18" r:id="rId30" xr:uid="{C8BED3F2-81F6-4AA6-84ED-18996181C7FD}"/>
+    <hyperlink ref="D19" r:id="rId31" xr:uid="{02C0E693-DC11-494B-B410-95217982373B}"/>
+    <hyperlink ref="D20" r:id="rId32" xr:uid="{A7D728B5-1825-4297-B1AC-7D7FE5890C3E}"/>
+    <hyperlink ref="D21" r:id="rId33" xr:uid="{5634882B-FCEA-44F8-B1DA-3C9E6E74F6E3}"/>
+    <hyperlink ref="D22" r:id="rId34" xr:uid="{66BCD681-8C02-497B-941E-3ECAE731AEF1}"/>
+    <hyperlink ref="D23" r:id="rId35" display="https://assets-barracuda-zoovu.azureedge.net/zoovu/c9988a81-6225-495e-9916-63507b5d2d52" xr:uid="{BE1BACC6-04E6-410D-9DCA-373BADED460A}"/>
+    <hyperlink ref="D24" r:id="rId36" display="https://assets-barracuda-zoovu.azureedge.net/zoovu/f9ede074-9c83-410f-afc0-5b3ada0d4856" xr:uid="{BF0C6E54-8295-4642-862C-2F5B83BA8FBC}"/>
+    <hyperlink ref="D25" r:id="rId37" xr:uid="{9069A94D-8425-4672-B8C0-57B34AAC43D4}"/>
+    <hyperlink ref="D26" r:id="rId38" xr:uid="{7F6C78C1-85A8-4F03-A793-1C961208BEA6}"/>
+    <hyperlink ref="D2" r:id="rId39" xr:uid="{DDBB2EE7-D674-4924-8E7D-6A88950572E3}"/>
+    <hyperlink ref="D3" r:id="rId40" xr:uid="{CE438329-BFBE-4B1B-AF1C-31E7BD2D94AA}"/>
+    <hyperlink ref="D4" r:id="rId41" xr:uid="{FA338553-EF85-4097-872D-5B82C6950237}"/>
+    <hyperlink ref="D5" r:id="rId42" xr:uid="{454154A0-D1D3-4BCB-BAB1-BA51B5DA9BDD}"/>
+    <hyperlink ref="D6" r:id="rId43" display="https://assets-barracuda-zoovu.azureedge.net/zoovu/132b01cc-9c95-4892-912f-64e65c2a71d0" xr:uid="{E8439CED-E6D4-433E-B7F1-05D369BDFDDA}"/>
+    <hyperlink ref="D7" r:id="rId44" display="https://assets-barracuda-zoovu.azureedge.net/zoovu/21bd4264-0b81-4daa-af12-c49864d722a2" xr:uid="{6410D3B1-4C6C-4A39-9F1C-1B767B93EE54}"/>
+    <hyperlink ref="D8" r:id="rId45" xr:uid="{6C8BB65A-F9C7-4B31-89AA-F3AEE1933CF2}"/>
+    <hyperlink ref="D9" r:id="rId46" xr:uid="{FDFF32F6-5719-4CFE-8CA4-4E36979A9AED}"/>
+    <hyperlink ref="D10" r:id="rId47" xr:uid="{0E333D1E-B3A8-49BC-818C-CBE48015CCC7}"/>
+    <hyperlink ref="D11" r:id="rId48" xr:uid="{608EF354-2CDF-40FD-A988-E071AEDEDC14}"/>
+    <hyperlink ref="D12" r:id="rId49" xr:uid="{9C43FED5-B639-48D7-88AC-2BC34DA8597F}"/>
+    <hyperlink ref="D13" r:id="rId50" display="https://assets-barracuda-zoovu.azureedge.net/zoovu/42823f08-0426-43ea-bd7b-39bc9cd0a001" xr:uid="{8693301A-2E67-486D-BDA2-FF1596A17577}"/>
+    <hyperlink ref="D17" r:id="rId51" display="https://assets-barracuda-zoovu.azureedge.net/zoovu/410eb56b-b1b6-48e7-9d66-de64912d72dc" xr:uid="{D2BB8838-82DD-4D96-A5FF-3394DD40BF9F}"/>
+    <hyperlink ref="D14" r:id="rId52" display="https://assets-barracuda-zoovu.azureedge.net/zoovu/fac7f86a-c529-4e61-9606-8d1792f57276" xr:uid="{1F0F088B-58D4-4E94-9811-D52467DE7D34}"/>
+    <hyperlink ref="D15" r:id="rId53" display="https://assets-barracuda-zoovu.azureedge.net/zoovu/138255fa-5f8c-48ab-baa2-ff10b2a19b98" xr:uid="{D3218EA2-66B9-4A8D-A513-77C484867503}"/>
+    <hyperlink ref="D16" r:id="rId54" xr:uid="{88C7C7CA-F208-487A-805C-F2435F6F3660}"/>
+    <hyperlink ref="D27" r:id="rId55" xr:uid="{D4B2729F-4EB7-4091-9B8F-2025E658A384}"/>
+    <hyperlink ref="D28" r:id="rId56" xr:uid="{1BB171EA-C394-485E-971E-00C4EB8E6858}"/>
+    <hyperlink ref="D29" r:id="rId57" xr:uid="{05DD7B07-C1D4-420A-B2AB-1119DCA8631C}"/>
+    <hyperlink ref="D30" r:id="rId58" xr:uid="{C6FD4B61-7B46-4581-8EF8-41E352131583}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId59"/>

</xml_diff>